<commit_message>
fixed seed data video urls
</commit_message>
<xml_diff>
--- a/app/assets/data/Sections.xlsx
+++ b/app/assets/data/Sections.xlsx
@@ -24,124 +24,124 @@
     <t>Introduction to Astronomy: Crash Course Astronomy #1</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/0rHUDWjR5gg?list=PL8dPuuaLjXtPAJr1ysd5yGIyiSFuh0mIL</t>
-  </si>
-  <si>
     <t>vid</t>
   </si>
   <si>
     <t>Naked Eye Observations: Crash Course Astronomy #2</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/L-Wtlev6suc?list=PL8dPuuaLjXtPAJr1ysd5yGIyiSFuh0mIL</t>
-  </si>
-  <si>
     <t>Cycles in the Sky: Crash Course Astronomy #3</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/01QWC-rZcfE?list=PL8dPuuaLjXtPAJr1ysd5yGIyiSFuh0mIL</t>
-  </si>
-  <si>
     <t>Moon Phases: Crash Course Astronomy #4</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/AQ5vty8f9Xc?list=PL8dPuuaLjXtPAJr1ysd5yGIyiSFuh0mIL</t>
-  </si>
-  <si>
     <t>Eclipses: Crash Course Astronomy #5</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/PRgua7xceDA?list=PL8dPuuaLjXtPAJr1ysd5yGIyiSFuh0mIL</t>
-  </si>
-  <si>
     <t>The Agricultural Revolution: Crash Course World History #1</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/Yocja_N5s1I?list=PLBDA2E52FB1EF80C9</t>
-  </si>
-  <si>
     <t>Indus Valley Civilization: Crash Course World History #2</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/n7ndRwqJYDM?list=PLBDA2E52FB1EF80C9</t>
-  </si>
-  <si>
     <t>Mesopotamia: Crash Course World History #3</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/sohXPx_XZ6Y?list=PLBDA2E52FB1EF80C9</t>
-  </si>
-  <si>
     <t>Ancient Egypt: Crash Course World History #4</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/Z3Wvw6BivVI?list=PLBDA2E52FB1EF80C9</t>
-  </si>
-  <si>
     <t>The Persians &amp; Greeks: Crash Course World History #5</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/Q-mkVSasZIM?list=PLBDA2E52FB1EF80C9</t>
-  </si>
-  <si>
     <t>The Nucleus: Crash Course Chemistry #1</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/FSyAehMdpyI?list=PL8dPuuaLjXtPHzzYuWy6fYEaX9mQQ8oGr</t>
-  </si>
-  <si>
     <t>Unit Conversion &amp; Significant Figures: Crash Course Chemistry #2</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/hQpQ0hxVNTg?list=PL8dPuuaLjXtPHzzYuWy6fYEaX9mQQ8oGr</t>
-  </si>
-  <si>
     <t>The Creation of Chemistry - The Fundamental Laws: Crash Course Chemistry #3</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/QiiyvzZBKT8?list=PL8dPuuaLjXtPHzzYuWy6fYEaX9mQQ8oGr</t>
-  </si>
-  <si>
     <t>The Periodic Table: Crash Course Chemistry #4</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/0RRVV4Diomg?list=PL8dPuuaLjXtPHzzYuWy6fYEaX9mQQ8oGr</t>
-  </si>
-  <si>
     <t>The Electron: Crash Course Chemistry #5</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/rcKilE9CdaA?list=PL8dPuuaLjXtPHzzYuWy6fYEaX9mQQ8oGr</t>
-  </si>
-  <si>
     <t>That's Why Carbon Is A Tramp: Crash Course Biology #1</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/QnQe0xW_JY4?list=PL3EED4C1D684D3ADF</t>
-  </si>
-  <si>
     <t>Water - Liquid Awesome: Crash Course Biology #2</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/HVT3Y3_gHGg?list=PL3EED4C1D684D3ADF</t>
-  </si>
-  <si>
     <t>Biological Molecules - You Are What You Eat: Crash Course Biology #3</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/H8WJ2KENlK0?list=PL3EED4C1D684D3ADF</t>
-  </si>
-  <si>
     <t>Eukaryopolis - The City of Animal Cells: Crash Course Biology #4</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/cj8dDTHGJBY?list=PL3EED4C1D684D3ADF</t>
-  </si>
-  <si>
     <t>In Da Club - Membranes &amp; Transport: Crash Course Biology #5</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/dPKvHrD1eS4?list=PL3EED4C1D684D3ADF</t>
+    <t>https://www.youtube.com/watch?v=0rHUDWjR5gg&amp;list=PL8dPuuaLjXtPAJr1ysd5yGIyiSFuh0mIL</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=L-Wtlev6suc&amp;list=PL8dPuuaLjXtPAJr1ysd5yGIyiSFuh0mIL&amp;index=2</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=01QWC-rZcfE&amp;list=PL8dPuuaLjXtPAJr1ysd5yGIyiSFuh0mIL&amp;index=3</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=AQ5vty8f9Xc&amp;list=PL8dPuuaLjXtPAJr1ysd5yGIyiSFuh0mIL&amp;index=4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PRgua7xceDA&amp;index=5&amp;list=PL8dPuuaLjXtPAJr1ysd5yGIyiSFuh0mIL</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Yocja_N5s1I&amp;list=PLBDA2E52FB1EF80C9</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=n7ndRwqJYDM&amp;index=2&amp;list=PLBDA2E52FB1EF80C9</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sohXPx_XZ6Y&amp;index=3&amp;list=PLBDA2E52FB1EF80C9</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Z3Wvw6BivVI&amp;index=4&amp;list=PLBDA2E52FB1EF80C9</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Q-mkVSasZIM&amp;list=PLBDA2E52FB1EF80C9&amp;index=5</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=FSyAehMdpyI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=hQpQ0hxVNTg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=QiiyvzZBKT8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=0RRVV4Diomg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rcKilE9CdaA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=QnQe0xW_JY4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=HVT3Y3_gHGg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=H8WJ2KENlK0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cj8dDTHGJBY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=dPKvHrD1eS4</t>
   </si>
 </sst>
 </file>
@@ -190,17 +190,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -468,7 +476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -479,7 +487,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -492,10 +500,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1">
         <v>1</v>
@@ -506,13 +514,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -523,13 +531,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -540,13 +548,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -557,13 +565,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -574,13 +582,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -591,13 +599,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -608,13 +616,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -625,13 +633,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -642,13 +650,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -659,13 +667,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -676,13 +684,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>7</v>
@@ -693,13 +701,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>8</v>
@@ -710,13 +718,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <v>8</v>
@@ -727,13 +735,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>9</v>
@@ -744,13 +752,13 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -761,13 +769,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>10</v>
@@ -778,13 +786,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>11</v>
@@ -795,13 +803,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <v>11</v>
@@ -812,13 +820,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>11</v>
@@ -832,10 +840,10 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21">
         <v>12</v>
@@ -846,13 +854,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22">
         <v>12</v>

</xml_diff>